<commit_message>
resolve invalid json bug
</commit_message>
<xml_diff>
--- a/banchmark/History.xlsx
+++ b/banchmark/History.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F86"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="E27" sqref="E27"/>
@@ -1598,6 +1598,1678 @@
         </is>
       </c>
     </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2025-05-29 22:02:39</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>https://www.google.com</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>GET</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Rata de iesire</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>100 requesturi =&gt; 113.03 req/s
+200 requesturi =&gt; 198.15 req/s
+400 requesturi =&gt; 124.03 req/s
+Output Rate: 198.15 req/s</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2025-05-29 22:02:55</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>https://www.google.com</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>GET</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Rata de iesire</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>100 requesturi =&gt; 117.22 req/s
+200 requesturi =&gt; 215.68 req/s
+400 requesturi =&gt; 112.51 req/s
+Output Rate: 215.68 req/s</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2025-05-29 22:30:18</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>https://www.google.com</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>GET</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Timp de raspuns</t>
+        </is>
+      </c>
+      <c r="E38" t="n">
+        <v>100</v>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Timp mediu: 468.74 ms
+Timp minim: 426.16 ms
+Timp maxim: 684.22 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2025-05-29 22:31:53</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>https://www.google.com</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>GET</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Timp de raspuns</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
+        <v>500</v>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Timp mediu: 632.20 ms
+Timp minim: 454.03 ms
+Timp maxim: 1650.67 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2025-05-29 22:32:20</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>https://www.google.com</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>GET</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Timp de raspuns</t>
+        </is>
+      </c>
+      <c r="E40" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Timp mediu: 1537.27 ms
+Timp minim: 460.36 ms
+Timp maxim: 3178.07 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2025-05-29 22:33:11</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>https://www.google.com</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>GET</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Timp de raspuns</t>
+        </is>
+      </c>
+      <c r="E41" t="n">
+        <v>5000</v>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Timp mediu: 2993.38 ms
+Timp minim: 433.22 ms
+Timp maxim: 7097.58 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2025-05-29 22:34:37</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>https://www.google.com</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>GET</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Rata de iesire</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>100 requesturi =&gt; 133.06 req/s
+200 requesturi =&gt; 279.56 req/s
+400 requesturi =&gt; 171.30 req/s
+Output Rate: 279.56 req/s</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2025-05-29 22:47:09</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>http://localhost:8080/</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>GET</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Timp de raspuns</t>
+        </is>
+      </c>
+      <c r="E43" t="n">
+        <v>100</v>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Timp mediu: 2083.18 ms
+Timp minim: 2035.23 ms
+Timp maxim: 2132.86 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2025-05-29 22:48:50</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>http://localhost:8080/</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>GET</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Timp de raspuns</t>
+        </is>
+      </c>
+      <c r="E44" t="n">
+        <v>500</v>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>Timp mediu: 2292.91 ms
+Timp minim: 2027.29 ms
+Timp maxim: 2676.56 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2025-05-29 22:49:20</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>http://localhost:8080/</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>GET</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Timp de raspuns</t>
+        </is>
+      </c>
+      <c r="E45" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Timp mediu: 2460.19 ms
+Timp minim: 2035.49 ms
+Timp maxim: 3262.20 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2025-05-29 22:50:04</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>http://localhost:8080/</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>GET</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Timp de raspuns</t>
+        </is>
+      </c>
+      <c r="E46" t="n">
+        <v>5000</v>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Timp mediu: 2175.15 ms
+Timp minim: 2018.16 ms
+Timp maxim: 3623.60 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2025-05-29 22:51:08</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>http://localhost:8080/</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>GET</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Timp de raspuns</t>
+        </is>
+      </c>
+      <c r="E47" t="n">
+        <v>10000</v>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Timp mediu: 2092.16 ms
+Timp minim: 2017.05 ms
+Timp maxim: 3585.68 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2025-05-29 22:57:08</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>http://localhost:8080/</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>POST</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Timp de raspuns</t>
+        </is>
+      </c>
+      <c r="E48" t="n">
+        <v>100</v>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Timp mediu: 2087.71 ms
+Timp minim: 2028.89 ms
+Timp maxim: 2134.23 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2025-05-29 22:58:11</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>http://localhost:8080/</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>POST</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Timp de raspuns</t>
+        </is>
+      </c>
+      <c r="E49" t="n">
+        <v>500</v>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Timp mediu: 2248.85 ms
+Timp minim: 2027.49 ms
+Timp maxim: 2617.29 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2025-05-29 22:58:41</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>http://localhost:8080/</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>POST</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Timp de raspuns</t>
+        </is>
+      </c>
+      <c r="E50" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>Timp mediu: 2365.52 ms
+Timp minim: 2039.75 ms
+Timp maxim: 3172.35 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2025-05-29 22:59:34</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>http://localhost:8080/</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>POST</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Timp de raspuns</t>
+        </is>
+      </c>
+      <c r="E51" t="n">
+        <v>5000</v>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Timp mediu: 2150.16 ms
+Timp minim: 2012.59 ms
+Timp maxim: 3699.68 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2025-05-29 23:01:34</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>http://localhost:8080/</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>POST</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Timp de raspuns</t>
+        </is>
+      </c>
+      <c r="E52" t="n">
+        <v>10000</v>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>Timp mediu: 2095.16 ms
+Timp minim: 2012.06 ms
+Timp maxim: 3250.86 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2025-05-29 23:06:42</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>http://localhost:8080/</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>GET</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Rata de iesire</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>100 requesturi =&gt; 45.54 req/s
+200 requesturi =&gt; 83.86 req/s
+400 requesturi =&gt; 137.28 req/s
+800 requesturi =&gt; 217.70 req/s
+1600 requesturi =&gt; 339.05 req/s
+3200 requesturi =&gt; 545.09 req/s
+6400 requesturi =&gt; 593.33 req/s
+12800 requesturi =&gt; 613.23 req/s
+Output Rate: 613.23 req/s</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2025-05-29 23:12:17</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>http://localhost:8080/</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>POST</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Rata de iesire</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>100 requesturi =&gt; 45.17 req/s
+200 requesturi =&gt; 84.31 req/s
+400 requesturi =&gt; 132.48 req/s
+800 requesturi =&gt; 237.16 req/s
+1600 requesturi =&gt; 350.60 req/s
+3200 requesturi =&gt; 453.51 req/s
+6400 requesturi =&gt; 583.17 req/s
+12800 requesturi =&gt; 505.62 req/s
+Output Rate: 583.17 req/s</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2025-05-29 23:23:14</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>http://localhost:8080/api/users/me</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>GET</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Timp de raspuns</t>
+        </is>
+      </c>
+      <c r="E55" t="n">
+        <v>10</v>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>Timp mediu: 5.41 ms
+Timp minim: 3.53 ms
+Timp maxim: 7.72 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2025-05-29 23:26:02</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>http://localhost:8080/api/users/me</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>GET</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Timp de raspuns</t>
+        </is>
+      </c>
+      <c r="E56" t="n">
+        <v>100</v>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>Timp mediu: 12.83 ms
+Timp minim: 4.54 ms
+Timp maxim: 21.82 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2025-05-29 23:27:21</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>http://localhost:8080/api/users/me</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>GET</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Timp de raspuns</t>
+        </is>
+      </c>
+      <c r="E57" t="n">
+        <v>500</v>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>Timp mediu: 14.21 ms
+Timp minim: 4.76 ms
+Timp maxim: 25.67 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2025-05-29 23:27:53</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>http://localhost:8080/api/users/mee</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>GET</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Timp de raspuns</t>
+        </is>
+      </c>
+      <c r="E58" t="n">
+        <v>500</v>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>Timp mediu: 46.93 ms
+Timp minim: 12.01 ms
+Timp maxim: 78.68 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2025-05-29 23:28:02</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>http://localhost:8080/api/users/mee</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>GET</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Timp de raspuns</t>
+        </is>
+      </c>
+      <c r="E59" t="n">
+        <v>500</v>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>Timp mediu: 47.61 ms
+Timp minim: 10.30 ms
+Timp maxim: 84.42 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2025-05-29 23:28:06</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>http://localhost:8080/api/users/meeeeee</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>GET</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Timp de raspuns</t>
+        </is>
+      </c>
+      <c r="E60" t="n">
+        <v>500</v>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>Timp mediu: 45.39 ms
+Timp minim: 8.23 ms
+Timp maxim: 71.10 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2025-05-29 23:28:20</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>http://localhost:8080/api/users/me</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>GET</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Rata de iesire</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>100 requesturi =&gt; 887.81 req/s
+200 requesturi =&gt; 909.89 req/s
+Output Rate: 909.89 req/s</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>2025-05-29 23:28:26</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>http://localhost:8080/api/users/me</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>GET</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Rata de iesire</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>100 requesturi =&gt; 911.69 req/s
+200 requesturi =&gt; 921.81 req/s
+Output Rate: 921.81 req/s</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>2025-05-29 23:28:29</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>http://localhost:8080/api/users/me</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>GET</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Rata de iesire</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>100 requesturi =&gt; 708.34 req/s
+200 requesturi =&gt; 861.53 req/s
+400 requesturi =&gt; 929.68 req/s
+800 requesturi =&gt; 918.46 req/s
+Output Rate: 929.68 req/s</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>2025-05-29 23:29:53</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>http://localhost:8080/api/planes/add</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>POST</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Timp de raspuns</t>
+        </is>
+      </c>
+      <c r="E64" t="n">
+        <v>1</v>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>Timp mediu: 4.57 ms
+Timp minim: 4.57 ms
+Timp maxim: 4.57 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>2025-05-29 23:30:21</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>http://localhost:8080/api/planes/add</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>POST</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Timp de raspuns</t>
+        </is>
+      </c>
+      <c r="E65" t="n">
+        <v>1</v>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>Timp mediu: 5.18 ms
+Timp minim: 5.18 ms
+Timp maxim: 5.18 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>2025-05-29 23:32:31</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>http://localhost:8080/login?email=maryuscostescu558@yahoo.com&amp;password=12345678</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>POST</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Timp de raspuns</t>
+        </is>
+      </c>
+      <c r="E66" t="n">
+        <v>1</v>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>Timp mediu: 88.77 ms
+Timp minim: 88.77 ms
+Timp maxim: 88.77 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>2025-05-29 23:32:35</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>http://localhost:8080/login?email=maryuscostescu558@yahoo.com&amp;password=12345678</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>POST</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>Timp de raspuns</t>
+        </is>
+      </c>
+      <c r="E67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>Timp mediu: 75.70 ms
+Timp minim: 75.70 ms
+Timp maxim: 75.70 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>2025-05-29 23:32:36</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>http://localhost:8080/login?email=maryuscostescu558@yahoo.com&amp;password=12345678</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>POST</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Timp de raspuns</t>
+        </is>
+      </c>
+      <c r="E68" t="n">
+        <v>1</v>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>Timp mediu: 77.50 ms
+Timp minim: 77.50 ms
+Timp maxim: 77.50 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>2025-05-29 23:32:37</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>http://localhost:8080/login?email=maryuscostescu558@yahoo.com&amp;password=12345678</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>POST</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>Timp de raspuns</t>
+        </is>
+      </c>
+      <c r="E69" t="n">
+        <v>1</v>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>Timp mediu: 75.28 ms
+Timp minim: 75.28 ms
+Timp maxim: 75.28 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>2025-05-29 23:32:53</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>http://localhost:8080/api/planes/add</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>POST</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>Timp de raspuns</t>
+        </is>
+      </c>
+      <c r="E70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>Timp mediu: 4.67 ms
+Timp minim: 4.67 ms
+Timp maxim: 4.67 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>2025-05-29 23:33:55</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>http://localhost:8080/api/planes/add</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>POST</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>Timp de raspuns</t>
+        </is>
+      </c>
+      <c r="E71" t="n">
+        <v>1</v>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>Timp mediu: 5.03 ms
+Timp minim: 5.03 ms
+Timp maxim: 5.03 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>2025-05-29 23:33:56</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>http://localhost:8080/api/planes/add</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>POST</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Timp de raspuns</t>
+        </is>
+      </c>
+      <c r="E72" t="n">
+        <v>1</v>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>Timp mediu: 4.01 ms
+Timp minim: 4.01 ms
+Timp maxim: 4.01 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>2025-05-29 23:33:56</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>http://localhost:8080/api/planes/add</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>POST</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>Timp de raspuns</t>
+        </is>
+      </c>
+      <c r="E73" t="n">
+        <v>1</v>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>Timp mediu: 4.09 ms
+Timp minim: 4.09 ms
+Timp maxim: 4.09 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>2025-05-29 23:35:09</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>http://localhost:8080/login?email=maryuscostescu558@yahoo.com&amp;password=12345678</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>GET</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>Timp de raspuns</t>
+        </is>
+      </c>
+      <c r="E74" t="n">
+        <v>10</v>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>Timp mediu: 15.31 ms
+Timp minim: 13.84 ms
+Timp maxim: 18.34 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>2025-05-29 23:35:20</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>http://localhost:8080/login?email=maryuscostescu558@yahoo.com&amp;password=12345678</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>POST</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>Timp de raspuns</t>
+        </is>
+      </c>
+      <c r="E75" t="n">
+        <v>1</v>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>Timp mediu: 82.18 ms
+Timp minim: 82.18 ms
+Timp maxim: 82.18 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>2025-05-29 23:35:21</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>http://localhost:8080/login?email=maryuscostescu558@yahoo.com&amp;password=12345678</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>POST</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>Timp de raspuns</t>
+        </is>
+      </c>
+      <c r="E76" t="n">
+        <v>1</v>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>Timp mediu: 79.13 ms
+Timp minim: 79.13 ms
+Timp maxim: 79.13 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>2025-05-29 23:35:46</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>http://localhost:8080/api/planes/add</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>POST</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>Timp de raspuns</t>
+        </is>
+      </c>
+      <c r="E77" t="n">
+        <v>1</v>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>Timp mediu: 4.30 ms
+Timp minim: 4.30 ms
+Timp maxim: 4.30 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>2025-05-29 23:35:47</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>http://localhost:8080/api/planes/add</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>POST</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>Timp de raspuns</t>
+        </is>
+      </c>
+      <c r="E78" t="n">
+        <v>1</v>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>Timp mediu: 4.48 ms
+Timp minim: 4.48 ms
+Timp maxim: 4.48 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>2025-05-29 23:35:49</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>http://localhost:8080/api/planes/add</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>GET</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>Timp de raspuns</t>
+        </is>
+      </c>
+      <c r="E79" t="n">
+        <v>1</v>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>Timp mediu: 4.48 ms
+Timp minim: 4.48 ms
+Timp maxim: 4.48 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>2025-05-29 23:35:50</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>http://localhost:8080/api/planes/add</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>GET</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>Timp de raspuns</t>
+        </is>
+      </c>
+      <c r="E80" t="n">
+        <v>1</v>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>Timp mediu: 4.91 ms
+Timp minim: 4.91 ms
+Timp maxim: 4.91 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>2025-05-29 23:40:27</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>http://localhost:8080/api/users/me</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>GET</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>Timp de raspuns</t>
+        </is>
+      </c>
+      <c r="E81" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>Timp mediu: 14.05 ms
+Timp minim: 5.09 ms
+Timp maxim: 25.53 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>2025-05-29 23:40:52</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>http://localhost:8080/api/users/me</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>GET</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>Timp de raspuns</t>
+        </is>
+      </c>
+      <c r="E82" t="n">
+        <v>5000</v>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>Timp mediu: 61.45 ms
+Timp minim: 3.52 ms
+Timp maxim: 318.30 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>2025-05-29 23:41:24</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>http://localhost:8080/api/users/me</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>GET</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>Timp de raspuns</t>
+        </is>
+      </c>
+      <c r="E83" t="n">
+        <v>10000</v>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>Timp mediu: 174.07 ms
+Timp minim: 2.86 ms
+Timp maxim: 796.71 ms</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>2025-05-29 23:44:36</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>http://localhost:8080/api/users/me</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>GET</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>Rata de iesire</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>100 requesturi =&gt; 813.89 req/s
+200 requesturi =&gt; 815.18 req/s
+Output Rate: 815.18 req/s</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>2025-05-29 23:44:38</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>http://localhost:8080/api/users/me</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>GET</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>Rata de iesire</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>100 requesturi =&gt; 817.42 req/s
+200 requesturi =&gt; 749.43 req/s
+Output Rate: 817.42 req/s</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>2025-05-29 23:44:39</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>http://localhost:8080/api/users/me</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>GET</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>Rata de iesire</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>100 requesturi =&gt; 784.31 req/s
+200 requesturi =&gt; 833.80 req/s
+400 requesturi =&gt; 818.28 req/s
+Output Rate: 833.80 req/s</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>